<commit_message>
Cambiado el nombre de requirements.tsx, añadadido archivo con emails y subido al gitignore
</commit_message>
<xml_diff>
--- a/data/precios_creatina.xlsx
+++ b/data/precios_creatina.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D160"/>
+  <dimension ref="A1:D161"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3621,7 +3621,7 @@
     </row>
     <row r="160">
       <c r="A160" s="2" t="n">
-        <v>45958.79050087265</v>
+        <v>45958.79050086805</v>
       </c>
       <c r="B160" t="inlineStr">
         <is>
@@ -3634,6 +3634,26 @@
         </is>
       </c>
       <c r="D160" t="inlineStr">
+        <is>
+          <t>14,00€</t>
+        </is>
+      </c>
+    </row>
+    <row r="161">
+      <c r="A161" s="2" t="n">
+        <v>45964.36348250412</v>
+      </c>
+      <c r="B161" t="inlineStr">
+        <is>
+          <t>CREATINA MONOHIDRATO EN POLVO</t>
+        </is>
+      </c>
+      <c r="C161" t="inlineStr">
+        <is>
+          <t>1Kg</t>
+        </is>
+      </c>
+      <c r="D161" t="inlineStr">
         <is>
           <t>14,00€</t>
         </is>

</xml_diff>

<commit_message>
Mejora para mostrar mas información sobre los precios
</commit_message>
<xml_diff>
--- a/data/precios_creatina.xlsx
+++ b/data/precios_creatina.xlsx
@@ -16,9 +16,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="yyyy-mm-dd h:mm:ss"/>
     <numFmt numFmtId="165" formatCode="YYYY-MM-DD HH:MM:SS"/>
+    <numFmt numFmtId="166" formatCode="yyyy-mm-dd"/>
+    <numFmt numFmtId="167" formatCode="YYYY-MM-DD"/>
   </numFmts>
   <fonts count="2">
     <font>
@@ -58,12 +60,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -429,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D161"/>
+  <dimension ref="A1:F188"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -458,6 +461,16 @@
           <t>precio</t>
         </is>
       </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>precio_num</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>fecha_dia</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="2" t="n">
@@ -478,6 +491,12 @@
           <t>12,88€</t>
         </is>
       </c>
+      <c r="E2" t="n">
+        <v>12.88</v>
+      </c>
+      <c r="F2" s="3" t="n">
+        <v>45804</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="n">
@@ -498,6 +517,12 @@
           <t>12,88€</t>
         </is>
       </c>
+      <c r="E3" t="n">
+        <v>12.88</v>
+      </c>
+      <c r="F3" s="3" t="n">
+        <v>45804</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="2" t="n">
@@ -518,6 +543,12 @@
           <t>15,41€</t>
         </is>
       </c>
+      <c r="E4" t="n">
+        <v>15.41</v>
+      </c>
+      <c r="F4" s="3" t="n">
+        <v>45805</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="2" t="n">
@@ -538,6 +569,12 @@
           <t>12,88€</t>
         </is>
       </c>
+      <c r="E5" t="n">
+        <v>12.88</v>
+      </c>
+      <c r="F5" s="3" t="n">
+        <v>45806</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="2" t="n">
@@ -558,6 +595,12 @@
           <t>12,88€</t>
         </is>
       </c>
+      <c r="E6" t="n">
+        <v>12.88</v>
+      </c>
+      <c r="F6" s="3" t="n">
+        <v>45806</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="2" t="n">
@@ -578,6 +621,12 @@
           <t>15,41€</t>
         </is>
       </c>
+      <c r="E7" t="n">
+        <v>15.41</v>
+      </c>
+      <c r="F7" s="3" t="n">
+        <v>45807</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="2" t="n">
@@ -598,6 +647,12 @@
           <t>15,41€</t>
         </is>
       </c>
+      <c r="E8" t="n">
+        <v>15.41</v>
+      </c>
+      <c r="F8" s="3" t="n">
+        <v>45808</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="2" t="n">
@@ -618,6 +673,12 @@
           <t>15,41€</t>
         </is>
       </c>
+      <c r="E9" t="n">
+        <v>15.41</v>
+      </c>
+      <c r="F9" s="3" t="n">
+        <v>45809</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="2" t="n">
@@ -638,6 +699,12 @@
           <t>15,41€</t>
         </is>
       </c>
+      <c r="E10" t="n">
+        <v>15.41</v>
+      </c>
+      <c r="F10" s="3" t="n">
+        <v>45810</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="2" t="n">
@@ -658,6 +725,12 @@
           <t>15,41€</t>
         </is>
       </c>
+      <c r="E11" t="n">
+        <v>15.41</v>
+      </c>
+      <c r="F11" s="3" t="n">
+        <v>45811</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="2" t="n">
@@ -678,6 +751,12 @@
           <t>12,88€</t>
         </is>
       </c>
+      <c r="E12" t="n">
+        <v>12.88</v>
+      </c>
+      <c r="F12" s="3" t="n">
+        <v>45812</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" s="2" t="n">
@@ -698,6 +777,12 @@
           <t>15,41€</t>
         </is>
       </c>
+      <c r="E13" t="n">
+        <v>15.41</v>
+      </c>
+      <c r="F13" s="3" t="n">
+        <v>45813</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" s="2" t="n">
@@ -718,6 +803,12 @@
           <t>15,41€</t>
         </is>
       </c>
+      <c r="E14" t="n">
+        <v>15.41</v>
+      </c>
+      <c r="F14" s="3" t="n">
+        <v>45814</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" s="2" t="n">
@@ -738,6 +829,12 @@
           <t>15,41€</t>
         </is>
       </c>
+      <c r="E15" t="n">
+        <v>15.41</v>
+      </c>
+      <c r="F15" s="3" t="n">
+        <v>45815</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" s="2" t="n">
@@ -758,6 +855,12 @@
           <t>15,41€</t>
         </is>
       </c>
+      <c r="E16" t="n">
+        <v>15.41</v>
+      </c>
+      <c r="F16" s="3" t="n">
+        <v>45816</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" s="2" t="n">
@@ -778,6 +881,12 @@
           <t>15,41€</t>
         </is>
       </c>
+      <c r="E17" t="n">
+        <v>15.41</v>
+      </c>
+      <c r="F17" s="3" t="n">
+        <v>45817</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" s="2" t="n">
@@ -798,6 +907,12 @@
           <t>15,41€</t>
         </is>
       </c>
+      <c r="E18" t="n">
+        <v>15.41</v>
+      </c>
+      <c r="F18" s="3" t="n">
+        <v>45818</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" s="2" t="n">
@@ -818,6 +933,12 @@
           <t>15,41€</t>
         </is>
       </c>
+      <c r="E19" t="n">
+        <v>15.41</v>
+      </c>
+      <c r="F19" s="3" t="n">
+        <v>45833</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" s="2" t="n">
@@ -838,6 +959,12 @@
           <t>15,41€</t>
         </is>
       </c>
+      <c r="E20" t="n">
+        <v>15.41</v>
+      </c>
+      <c r="F20" s="3" t="n">
+        <v>45833</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" s="2" t="n">
@@ -858,6 +985,12 @@
           <t>15,41€</t>
         </is>
       </c>
+      <c r="E21" t="n">
+        <v>15.41</v>
+      </c>
+      <c r="F21" s="3" t="n">
+        <v>45833</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" s="2" t="n">
@@ -878,6 +1011,12 @@
           <t>15,41€</t>
         </is>
       </c>
+      <c r="E22" t="n">
+        <v>15.41</v>
+      </c>
+      <c r="F22" s="3" t="n">
+        <v>45833</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" s="2" t="n">
@@ -898,6 +1037,12 @@
           <t>15,41€</t>
         </is>
       </c>
+      <c r="E23" t="n">
+        <v>15.41</v>
+      </c>
+      <c r="F23" s="3" t="n">
+        <v>45833</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" s="2" t="n">
@@ -918,6 +1063,12 @@
           <t>15,41€</t>
         </is>
       </c>
+      <c r="E24" t="n">
+        <v>15.41</v>
+      </c>
+      <c r="F24" s="3" t="n">
+        <v>45833</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" s="2" t="n">
@@ -938,6 +1089,12 @@
           <t>15,41€</t>
         </is>
       </c>
+      <c r="E25" t="n">
+        <v>15.41</v>
+      </c>
+      <c r="F25" s="3" t="n">
+        <v>45833</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" s="2" t="n">
@@ -958,6 +1115,12 @@
           <t>15,41€</t>
         </is>
       </c>
+      <c r="E26" t="n">
+        <v>15.41</v>
+      </c>
+      <c r="F26" s="3" t="n">
+        <v>45833</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" s="2" t="n">
@@ -978,6 +1141,12 @@
           <t>15,41€</t>
         </is>
       </c>
+      <c r="E27" t="n">
+        <v>15.41</v>
+      </c>
+      <c r="F27" s="3" t="n">
+        <v>45833</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28" s="2" t="n">
@@ -998,6 +1167,12 @@
           <t>15,41€</t>
         </is>
       </c>
+      <c r="E28" t="n">
+        <v>15.41</v>
+      </c>
+      <c r="F28" s="3" t="n">
+        <v>45833</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" s="2" t="n">
@@ -1018,6 +1193,12 @@
           <t>15,41€</t>
         </is>
       </c>
+      <c r="E29" t="n">
+        <v>15.41</v>
+      </c>
+      <c r="F29" s="3" t="n">
+        <v>45833</v>
+      </c>
     </row>
     <row r="30">
       <c r="A30" s="2" t="n">
@@ -1038,6 +1219,12 @@
           <t>15,41€</t>
         </is>
       </c>
+      <c r="E30" t="n">
+        <v>15.41</v>
+      </c>
+      <c r="F30" s="3" t="n">
+        <v>45833</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31" s="2" t="n">
@@ -1058,6 +1245,12 @@
           <t>15,41€</t>
         </is>
       </c>
+      <c r="E31" t="n">
+        <v>15.41</v>
+      </c>
+      <c r="F31" s="3" t="n">
+        <v>45833</v>
+      </c>
     </row>
     <row r="32">
       <c r="A32" s="2" t="n">
@@ -1078,6 +1271,12 @@
           <t>15,41€</t>
         </is>
       </c>
+      <c r="E32" t="n">
+        <v>15.41</v>
+      </c>
+      <c r="F32" s="3" t="n">
+        <v>45833</v>
+      </c>
     </row>
     <row r="33">
       <c r="A33" s="2" t="n">
@@ -1098,6 +1297,12 @@
           <t>15,41€</t>
         </is>
       </c>
+      <c r="E33" t="n">
+        <v>15.41</v>
+      </c>
+      <c r="F33" s="3" t="n">
+        <v>45833</v>
+      </c>
     </row>
     <row r="34">
       <c r="A34" s="2" t="n">
@@ -1118,6 +1323,12 @@
           <t>15,41€</t>
         </is>
       </c>
+      <c r="E34" t="n">
+        <v>15.41</v>
+      </c>
+      <c r="F34" s="3" t="n">
+        <v>45833</v>
+      </c>
     </row>
     <row r="35">
       <c r="A35" s="2" t="n">
@@ -1138,6 +1349,12 @@
           <t>15,41€</t>
         </is>
       </c>
+      <c r="E35" t="n">
+        <v>15.41</v>
+      </c>
+      <c r="F35" s="3" t="n">
+        <v>45833</v>
+      </c>
     </row>
     <row r="36">
       <c r="A36" s="2" t="n">
@@ -1158,6 +1375,12 @@
           <t>15,41€</t>
         </is>
       </c>
+      <c r="E36" t="n">
+        <v>15.41</v>
+      </c>
+      <c r="F36" s="3" t="n">
+        <v>45833</v>
+      </c>
     </row>
     <row r="37">
       <c r="A37" s="2" t="n">
@@ -1178,6 +1401,12 @@
           <t>15,41€</t>
         </is>
       </c>
+      <c r="E37" t="n">
+        <v>15.41</v>
+      </c>
+      <c r="F37" s="3" t="n">
+        <v>45833</v>
+      </c>
     </row>
     <row r="38">
       <c r="A38" s="2" t="n">
@@ -1198,6 +1427,12 @@
           <t>12,88€</t>
         </is>
       </c>
+      <c r="E38" t="n">
+        <v>12.88</v>
+      </c>
+      <c r="F38" s="3" t="n">
+        <v>45834</v>
+      </c>
     </row>
     <row r="39">
       <c r="A39" s="2" t="n">
@@ -1218,6 +1453,12 @@
           <t>15,41€</t>
         </is>
       </c>
+      <c r="E39" t="n">
+        <v>15.41</v>
+      </c>
+      <c r="F39" s="3" t="n">
+        <v>45853</v>
+      </c>
     </row>
     <row r="40">
       <c r="A40" s="2" t="n">
@@ -1238,6 +1479,12 @@
           <t>15,41€</t>
         </is>
       </c>
+      <c r="E40" t="n">
+        <v>15.41</v>
+      </c>
+      <c r="F40" s="3" t="n">
+        <v>45853</v>
+      </c>
     </row>
     <row r="41">
       <c r="A41" s="2" t="n">
@@ -1258,6 +1505,12 @@
           <t>15,41€</t>
         </is>
       </c>
+      <c r="E41" t="n">
+        <v>15.41</v>
+      </c>
+      <c r="F41" s="3" t="n">
+        <v>45853</v>
+      </c>
     </row>
     <row r="42">
       <c r="A42" s="2" t="n">
@@ -1278,6 +1531,12 @@
           <t>15,41€</t>
         </is>
       </c>
+      <c r="E42" t="n">
+        <v>15.41</v>
+      </c>
+      <c r="F42" s="3" t="n">
+        <v>45853</v>
+      </c>
     </row>
     <row r="43">
       <c r="A43" s="2" t="n">
@@ -1298,6 +1557,12 @@
           <t>15,41€</t>
         </is>
       </c>
+      <c r="E43" t="n">
+        <v>15.41</v>
+      </c>
+      <c r="F43" s="3" t="n">
+        <v>45853</v>
+      </c>
     </row>
     <row r="44">
       <c r="A44" s="2" t="n">
@@ -1318,6 +1583,12 @@
           <t>15,41€</t>
         </is>
       </c>
+      <c r="E44" t="n">
+        <v>15.41</v>
+      </c>
+      <c r="F44" s="3" t="n">
+        <v>45853</v>
+      </c>
     </row>
     <row r="45">
       <c r="A45" s="2" t="n">
@@ -1338,6 +1609,12 @@
           <t>15,41€</t>
         </is>
       </c>
+      <c r="E45" t="n">
+        <v>15.41</v>
+      </c>
+      <c r="F45" s="3" t="n">
+        <v>45853</v>
+      </c>
     </row>
     <row r="46">
       <c r="A46" s="2" t="n">
@@ -1358,6 +1635,12 @@
           <t>15,41€</t>
         </is>
       </c>
+      <c r="E46" t="n">
+        <v>15.41</v>
+      </c>
+      <c r="F46" s="3" t="n">
+        <v>45853</v>
+      </c>
     </row>
     <row r="47">
       <c r="A47" s="2" t="n">
@@ -1378,6 +1661,12 @@
           <t>15,41€</t>
         </is>
       </c>
+      <c r="E47" t="n">
+        <v>15.41</v>
+      </c>
+      <c r="F47" s="3" t="n">
+        <v>45853</v>
+      </c>
     </row>
     <row r="48">
       <c r="A48" s="2" t="n">
@@ -1398,6 +1687,12 @@
           <t>15,41€</t>
         </is>
       </c>
+      <c r="E48" t="n">
+        <v>15.41</v>
+      </c>
+      <c r="F48" s="3" t="n">
+        <v>45853</v>
+      </c>
     </row>
     <row r="49">
       <c r="A49" s="2" t="n">
@@ -1418,6 +1713,12 @@
           <t>15,41€</t>
         </is>
       </c>
+      <c r="E49" t="n">
+        <v>15.41</v>
+      </c>
+      <c r="F49" s="3" t="n">
+        <v>45853</v>
+      </c>
     </row>
     <row r="50">
       <c r="A50" s="2" t="n">
@@ -1438,6 +1739,12 @@
           <t>15,41€</t>
         </is>
       </c>
+      <c r="E50" t="n">
+        <v>15.41</v>
+      </c>
+      <c r="F50" s="3" t="n">
+        <v>45853</v>
+      </c>
     </row>
     <row r="51">
       <c r="A51" s="2" t="n">
@@ -1458,6 +1765,12 @@
           <t>15,41€</t>
         </is>
       </c>
+      <c r="E51" t="n">
+        <v>15.41</v>
+      </c>
+      <c r="F51" s="3" t="n">
+        <v>45853</v>
+      </c>
     </row>
     <row r="52">
       <c r="A52" s="2" t="n">
@@ -1478,6 +1791,12 @@
           <t>15,41€</t>
         </is>
       </c>
+      <c r="E52" t="n">
+        <v>15.41</v>
+      </c>
+      <c r="F52" s="3" t="n">
+        <v>45853</v>
+      </c>
     </row>
     <row r="53">
       <c r="A53" s="2" t="n">
@@ -1498,6 +1817,12 @@
           <t>15,41€</t>
         </is>
       </c>
+      <c r="E53" t="n">
+        <v>15.41</v>
+      </c>
+      <c r="F53" s="3" t="n">
+        <v>45853</v>
+      </c>
     </row>
     <row r="54">
       <c r="A54" s="2" t="n">
@@ -1518,6 +1843,12 @@
           <t>15,41€</t>
         </is>
       </c>
+      <c r="E54" t="n">
+        <v>15.41</v>
+      </c>
+      <c r="F54" s="3" t="n">
+        <v>45853</v>
+      </c>
     </row>
     <row r="55">
       <c r="A55" s="2" t="n">
@@ -1538,6 +1869,12 @@
           <t>15,41€</t>
         </is>
       </c>
+      <c r="E55" t="n">
+        <v>15.41</v>
+      </c>
+      <c r="F55" s="3" t="n">
+        <v>45853</v>
+      </c>
     </row>
     <row r="56">
       <c r="A56" s="2" t="n">
@@ -1558,6 +1895,12 @@
           <t>15,41€</t>
         </is>
       </c>
+      <c r="E56" t="n">
+        <v>15.41</v>
+      </c>
+      <c r="F56" s="3" t="n">
+        <v>45853</v>
+      </c>
     </row>
     <row r="57">
       <c r="A57" s="2" t="n">
@@ -1578,6 +1921,12 @@
           <t>15,41€</t>
         </is>
       </c>
+      <c r="E57" t="n">
+        <v>15.41</v>
+      </c>
+      <c r="F57" s="3" t="n">
+        <v>45853</v>
+      </c>
     </row>
     <row r="58">
       <c r="A58" s="2" t="n">
@@ -1598,6 +1947,12 @@
           <t>15,41€</t>
         </is>
       </c>
+      <c r="E58" t="n">
+        <v>15.41</v>
+      </c>
+      <c r="F58" s="3" t="n">
+        <v>45853</v>
+      </c>
     </row>
     <row r="59">
       <c r="A59" s="2" t="n">
@@ -1618,6 +1973,12 @@
           <t>15,41€</t>
         </is>
       </c>
+      <c r="E59" t="n">
+        <v>15.41</v>
+      </c>
+      <c r="F59" s="3" t="n">
+        <v>45854</v>
+      </c>
     </row>
     <row r="60">
       <c r="A60" s="2" t="n">
@@ -1638,6 +1999,12 @@
           <t>15,41€</t>
         </is>
       </c>
+      <c r="E60" t="n">
+        <v>15.41</v>
+      </c>
+      <c r="F60" s="3" t="n">
+        <v>45854</v>
+      </c>
     </row>
     <row r="61">
       <c r="A61" s="2" t="n">
@@ -1658,6 +2025,12 @@
           <t>12,88€</t>
         </is>
       </c>
+      <c r="E61" t="n">
+        <v>12.88</v>
+      </c>
+      <c r="F61" s="3" t="n">
+        <v>45855</v>
+      </c>
     </row>
     <row r="62">
       <c r="A62" s="2" t="n">
@@ -1678,6 +2051,12 @@
           <t>12,88€</t>
         </is>
       </c>
+      <c r="E62" t="n">
+        <v>12.88</v>
+      </c>
+      <c r="F62" s="3" t="n">
+        <v>45855</v>
+      </c>
     </row>
     <row r="63">
       <c r="A63" s="2" t="n">
@@ -1698,6 +2077,12 @@
           <t>12,88€</t>
         </is>
       </c>
+      <c r="E63" t="n">
+        <v>12.88</v>
+      </c>
+      <c r="F63" s="3" t="n">
+        <v>45856</v>
+      </c>
     </row>
     <row r="64">
       <c r="A64" s="2" t="n">
@@ -1718,6 +2103,12 @@
           <t>15,41€</t>
         </is>
       </c>
+      <c r="E64" t="n">
+        <v>15.41</v>
+      </c>
+      <c r="F64" s="3" t="n">
+        <v>45857</v>
+      </c>
     </row>
     <row r="65">
       <c r="A65" s="2" t="n">
@@ -1738,6 +2129,12 @@
           <t>15,41€</t>
         </is>
       </c>
+      <c r="E65" t="n">
+        <v>15.41</v>
+      </c>
+      <c r="F65" s="3" t="n">
+        <v>45858</v>
+      </c>
     </row>
     <row r="66">
       <c r="A66" s="2" t="n">
@@ -1758,6 +2155,12 @@
           <t>15,41€</t>
         </is>
       </c>
+      <c r="E66" t="n">
+        <v>15.41</v>
+      </c>
+      <c r="F66" s="3" t="n">
+        <v>45859</v>
+      </c>
     </row>
     <row r="67">
       <c r="A67" s="2" t="n">
@@ -1778,6 +2181,12 @@
           <t>15,41€</t>
         </is>
       </c>
+      <c r="E67" t="n">
+        <v>15.41</v>
+      </c>
+      <c r="F67" s="3" t="n">
+        <v>45860</v>
+      </c>
     </row>
     <row r="68">
       <c r="A68" s="2" t="n">
@@ -1798,6 +2207,12 @@
           <t>12,88€</t>
         </is>
       </c>
+      <c r="E68" t="n">
+        <v>12.88</v>
+      </c>
+      <c r="F68" s="3" t="n">
+        <v>45861</v>
+      </c>
     </row>
     <row r="69">
       <c r="A69" s="2" t="n">
@@ -1818,6 +2233,12 @@
           <t>15,41€</t>
         </is>
       </c>
+      <c r="E69" t="n">
+        <v>15.41</v>
+      </c>
+      <c r="F69" s="3" t="n">
+        <v>45862</v>
+      </c>
     </row>
     <row r="70">
       <c r="A70" s="2" t="n">
@@ -1838,6 +2259,12 @@
           <t>15,41€</t>
         </is>
       </c>
+      <c r="E70" t="n">
+        <v>15.41</v>
+      </c>
+      <c r="F70" s="3" t="n">
+        <v>45863</v>
+      </c>
     </row>
     <row r="71">
       <c r="A71" s="2" t="n">
@@ -1858,6 +2285,12 @@
           <t>15,41€</t>
         </is>
       </c>
+      <c r="E71" t="n">
+        <v>15.41</v>
+      </c>
+      <c r="F71" s="3" t="n">
+        <v>45864</v>
+      </c>
     </row>
     <row r="72">
       <c r="A72" s="2" t="n">
@@ -1878,6 +2311,12 @@
           <t>15,41€</t>
         </is>
       </c>
+      <c r="E72" t="n">
+        <v>15.41</v>
+      </c>
+      <c r="F72" s="3" t="n">
+        <v>45865</v>
+      </c>
     </row>
     <row r="73">
       <c r="A73" s="2" t="n">
@@ -1898,6 +2337,12 @@
           <t>15,41€</t>
         </is>
       </c>
+      <c r="E73" t="n">
+        <v>15.41</v>
+      </c>
+      <c r="F73" s="3" t="n">
+        <v>45866</v>
+      </c>
     </row>
     <row r="74">
       <c r="A74" s="2" t="n">
@@ -1918,6 +2363,12 @@
           <t>14,75€</t>
         </is>
       </c>
+      <c r="E74" t="n">
+        <v>14.75</v>
+      </c>
+      <c r="F74" s="3" t="n">
+        <v>45867</v>
+      </c>
     </row>
     <row r="75">
       <c r="A75" s="2" t="n">
@@ -1938,6 +2389,12 @@
           <t>14,75€</t>
         </is>
       </c>
+      <c r="E75" t="n">
+        <v>14.75</v>
+      </c>
+      <c r="F75" s="3" t="n">
+        <v>45868</v>
+      </c>
     </row>
     <row r="76">
       <c r="A76" s="2" t="n">
@@ -1958,6 +2415,12 @@
           <t>15,41€</t>
         </is>
       </c>
+      <c r="E76" t="n">
+        <v>15.41</v>
+      </c>
+      <c r="F76" s="3" t="n">
+        <v>45869</v>
+      </c>
     </row>
     <row r="77">
       <c r="A77" s="2" t="n">
@@ -1978,6 +2441,12 @@
           <t>15,41€</t>
         </is>
       </c>
+      <c r="E77" t="n">
+        <v>15.41</v>
+      </c>
+      <c r="F77" s="3" t="n">
+        <v>45870</v>
+      </c>
     </row>
     <row r="78">
       <c r="A78" s="2" t="n">
@@ -1998,6 +2467,12 @@
           <t>15,41€</t>
         </is>
       </c>
+      <c r="E78" t="n">
+        <v>15.41</v>
+      </c>
+      <c r="F78" s="3" t="n">
+        <v>45871</v>
+      </c>
     </row>
     <row r="79">
       <c r="A79" s="2" t="n">
@@ -2018,6 +2493,12 @@
           <t>15,41€</t>
         </is>
       </c>
+      <c r="E79" t="n">
+        <v>15.41</v>
+      </c>
+      <c r="F79" s="3" t="n">
+        <v>45872</v>
+      </c>
     </row>
     <row r="80">
       <c r="A80" s="2" t="n">
@@ -2038,6 +2519,12 @@
           <t>14,75€</t>
         </is>
       </c>
+      <c r="E80" t="n">
+        <v>14.75</v>
+      </c>
+      <c r="F80" s="3" t="n">
+        <v>45873</v>
+      </c>
     </row>
     <row r="81">
       <c r="A81" s="2" t="n">
@@ -2058,6 +2545,12 @@
           <t>12,88€</t>
         </is>
       </c>
+      <c r="E81" t="n">
+        <v>12.88</v>
+      </c>
+      <c r="F81" s="3" t="n">
+        <v>45874</v>
+      </c>
     </row>
     <row r="82">
       <c r="A82" s="2" t="n">
@@ -2078,6 +2571,12 @@
           <t>12,88€</t>
         </is>
       </c>
+      <c r="E82" t="n">
+        <v>12.88</v>
+      </c>
+      <c r="F82" s="3" t="n">
+        <v>45875</v>
+      </c>
     </row>
     <row r="83">
       <c r="A83" s="2" t="n">
@@ -2098,6 +2597,12 @@
           <t>12,88€</t>
         </is>
       </c>
+      <c r="E83" t="n">
+        <v>12.88</v>
+      </c>
+      <c r="F83" s="3" t="n">
+        <v>45876</v>
+      </c>
     </row>
     <row r="84">
       <c r="A84" s="2" t="n">
@@ -2118,6 +2623,12 @@
           <t>15,41€</t>
         </is>
       </c>
+      <c r="E84" t="n">
+        <v>15.41</v>
+      </c>
+      <c r="F84" s="3" t="n">
+        <v>45877</v>
+      </c>
     </row>
     <row r="85">
       <c r="A85" s="2" t="n">
@@ -2138,6 +2649,12 @@
           <t>15,41€</t>
         </is>
       </c>
+      <c r="E85" t="n">
+        <v>15.41</v>
+      </c>
+      <c r="F85" s="3" t="n">
+        <v>45878</v>
+      </c>
     </row>
     <row r="86">
       <c r="A86" s="2" t="n">
@@ -2158,6 +2675,12 @@
           <t>15,41€</t>
         </is>
       </c>
+      <c r="E86" t="n">
+        <v>15.41</v>
+      </c>
+      <c r="F86" s="3" t="n">
+        <v>45879</v>
+      </c>
     </row>
     <row r="87">
       <c r="A87" s="2" t="n">
@@ -2178,6 +2701,12 @@
           <t>15,41€</t>
         </is>
       </c>
+      <c r="E87" t="n">
+        <v>15.41</v>
+      </c>
+      <c r="F87" s="3" t="n">
+        <v>45880</v>
+      </c>
     </row>
     <row r="88">
       <c r="A88" s="2" t="n">
@@ -2198,6 +2727,12 @@
           <t>14,75€</t>
         </is>
       </c>
+      <c r="E88" t="n">
+        <v>14.75</v>
+      </c>
+      <c r="F88" s="3" t="n">
+        <v>45881</v>
+      </c>
     </row>
     <row r="89">
       <c r="A89" s="2" t="n">
@@ -2218,6 +2753,12 @@
           <t>14,75€</t>
         </is>
       </c>
+      <c r="E89" t="n">
+        <v>14.75</v>
+      </c>
+      <c r="F89" s="3" t="n">
+        <v>45882</v>
+      </c>
     </row>
     <row r="90">
       <c r="A90" s="2" t="n">
@@ -2238,6 +2779,12 @@
           <t>14,75€</t>
         </is>
       </c>
+      <c r="E90" t="n">
+        <v>14.75</v>
+      </c>
+      <c r="F90" s="3" t="n">
+        <v>45883</v>
+      </c>
     </row>
     <row r="91">
       <c r="A91" s="2" t="n">
@@ -2258,6 +2805,12 @@
           <t>14,75€</t>
         </is>
       </c>
+      <c r="E91" t="n">
+        <v>14.75</v>
+      </c>
+      <c r="F91" s="3" t="n">
+        <v>45884</v>
+      </c>
     </row>
     <row r="92">
       <c r="A92" s="2" t="n">
@@ -2278,6 +2831,12 @@
           <t>15,41€</t>
         </is>
       </c>
+      <c r="E92" t="n">
+        <v>15.41</v>
+      </c>
+      <c r="F92" s="3" t="n">
+        <v>45885</v>
+      </c>
     </row>
     <row r="93">
       <c r="A93" s="2" t="n">
@@ -2298,6 +2857,12 @@
           <t>14,75€</t>
         </is>
       </c>
+      <c r="E93" t="n">
+        <v>14.75</v>
+      </c>
+      <c r="F93" s="3" t="n">
+        <v>45886</v>
+      </c>
     </row>
     <row r="94">
       <c r="A94" s="2" t="n">
@@ -2318,6 +2883,12 @@
           <t>14,75€</t>
         </is>
       </c>
+      <c r="E94" t="n">
+        <v>14.75</v>
+      </c>
+      <c r="F94" s="3" t="n">
+        <v>45887</v>
+      </c>
     </row>
     <row r="95">
       <c r="A95" s="2" t="n">
@@ -2338,6 +2909,12 @@
           <t>14,75€</t>
         </is>
       </c>
+      <c r="E95" t="n">
+        <v>14.75</v>
+      </c>
+      <c r="F95" s="3" t="n">
+        <v>45888</v>
+      </c>
     </row>
     <row r="96">
       <c r="A96" s="2" t="n">
@@ -2358,6 +2935,12 @@
           <t>14,75€</t>
         </is>
       </c>
+      <c r="E96" t="n">
+        <v>14.75</v>
+      </c>
+      <c r="F96" s="3" t="n">
+        <v>45889</v>
+      </c>
     </row>
     <row r="97">
       <c r="A97" s="2" t="n">
@@ -2378,6 +2961,12 @@
           <t>15,41€</t>
         </is>
       </c>
+      <c r="E97" t="n">
+        <v>15.41</v>
+      </c>
+      <c r="F97" s="3" t="n">
+        <v>45890</v>
+      </c>
     </row>
     <row r="98">
       <c r="A98" s="2" t="n">
@@ -2398,6 +2987,12 @@
           <t>14,75€</t>
         </is>
       </c>
+      <c r="E98" t="n">
+        <v>14.75</v>
+      </c>
+      <c r="F98" s="3" t="n">
+        <v>45891</v>
+      </c>
     </row>
     <row r="99">
       <c r="A99" s="2" t="n">
@@ -2418,6 +3013,12 @@
           <t>15,41€</t>
         </is>
       </c>
+      <c r="E99" t="n">
+        <v>15.41</v>
+      </c>
+      <c r="F99" s="3" t="n">
+        <v>45892</v>
+      </c>
     </row>
     <row r="100">
       <c r="A100" s="2" t="n">
@@ -2438,6 +3039,12 @@
           <t>14,75€</t>
         </is>
       </c>
+      <c r="E100" t="n">
+        <v>14.75</v>
+      </c>
+      <c r="F100" s="3" t="n">
+        <v>45893</v>
+      </c>
     </row>
     <row r="101">
       <c r="A101" s="2" t="n">
@@ -2458,6 +3065,12 @@
           <t>15,41€</t>
         </is>
       </c>
+      <c r="E101" t="n">
+        <v>15.41</v>
+      </c>
+      <c r="F101" s="3" t="n">
+        <v>45895</v>
+      </c>
     </row>
     <row r="102">
       <c r="A102" s="2" t="n">
@@ -2478,6 +3091,12 @@
           <t>15,41€</t>
         </is>
       </c>
+      <c r="E102" t="n">
+        <v>15.41</v>
+      </c>
+      <c r="F102" s="3" t="n">
+        <v>45896</v>
+      </c>
     </row>
     <row r="103">
       <c r="A103" s="2" t="n">
@@ -2498,6 +3117,12 @@
           <t>14,00€</t>
         </is>
       </c>
+      <c r="E103" t="n">
+        <v>14</v>
+      </c>
+      <c r="F103" s="3" t="n">
+        <v>45897</v>
+      </c>
     </row>
     <row r="104">
       <c r="A104" s="2" t="n">
@@ -2518,6 +3143,12 @@
           <t>15,41€</t>
         </is>
       </c>
+      <c r="E104" t="n">
+        <v>15.41</v>
+      </c>
+      <c r="F104" s="3" t="n">
+        <v>45898</v>
+      </c>
     </row>
     <row r="105">
       <c r="A105" s="2" t="n">
@@ -2538,6 +3169,12 @@
           <t>15,41€</t>
         </is>
       </c>
+      <c r="E105" t="n">
+        <v>15.41</v>
+      </c>
+      <c r="F105" s="3" t="n">
+        <v>45899</v>
+      </c>
     </row>
     <row r="106">
       <c r="A106" s="2" t="n">
@@ -2558,6 +3195,12 @@
           <t>14,00€</t>
         </is>
       </c>
+      <c r="E106" t="n">
+        <v>14</v>
+      </c>
+      <c r="F106" s="3" t="n">
+        <v>45900</v>
+      </c>
     </row>
     <row r="107">
       <c r="A107" s="2" t="n">
@@ -2578,6 +3221,12 @@
           <t>11,67€</t>
         </is>
       </c>
+      <c r="E107" t="n">
+        <v>11.67</v>
+      </c>
+      <c r="F107" s="3" t="n">
+        <v>45901</v>
+      </c>
     </row>
     <row r="108">
       <c r="A108" s="2" t="n">
@@ -2598,6 +3247,12 @@
           <t>14,00€</t>
         </is>
       </c>
+      <c r="E108" t="n">
+        <v>14</v>
+      </c>
+      <c r="F108" s="3" t="n">
+        <v>45902</v>
+      </c>
     </row>
     <row r="109">
       <c r="A109" s="2" t="n">
@@ -2618,6 +3273,12 @@
           <t>15,41€</t>
         </is>
       </c>
+      <c r="E109" t="n">
+        <v>15.41</v>
+      </c>
+      <c r="F109" s="3" t="n">
+        <v>45903</v>
+      </c>
     </row>
     <row r="110">
       <c r="A110" s="2" t="n">
@@ -2638,6 +3299,12 @@
           <t>15,41€</t>
         </is>
       </c>
+      <c r="E110" t="n">
+        <v>15.41</v>
+      </c>
+      <c r="F110" s="3" t="n">
+        <v>45904</v>
+      </c>
     </row>
     <row r="111">
       <c r="A111" s="2" t="n">
@@ -2658,6 +3325,12 @@
           <t>15,41€</t>
         </is>
       </c>
+      <c r="E111" t="n">
+        <v>15.41</v>
+      </c>
+      <c r="F111" s="3" t="n">
+        <v>45905</v>
+      </c>
     </row>
     <row r="112">
       <c r="A112" s="2" t="n">
@@ -2678,6 +3351,12 @@
           <t>15,41€</t>
         </is>
       </c>
+      <c r="E112" t="n">
+        <v>15.41</v>
+      </c>
+      <c r="F112" s="3" t="n">
+        <v>45906</v>
+      </c>
     </row>
     <row r="113">
       <c r="A113" s="2" t="n">
@@ -2698,6 +3377,12 @@
           <t>14,00€</t>
         </is>
       </c>
+      <c r="E113" t="n">
+        <v>14</v>
+      </c>
+      <c r="F113" s="3" t="n">
+        <v>45907</v>
+      </c>
     </row>
     <row r="114">
       <c r="A114" s="2" t="n">
@@ -2718,6 +3403,12 @@
           <t>15,41€</t>
         </is>
       </c>
+      <c r="E114" t="n">
+        <v>15.41</v>
+      </c>
+      <c r="F114" s="3" t="n">
+        <v>45908</v>
+      </c>
     </row>
     <row r="115">
       <c r="A115" s="2" t="n">
@@ -2738,6 +3429,12 @@
           <t>11,67€</t>
         </is>
       </c>
+      <c r="E115" t="n">
+        <v>11.67</v>
+      </c>
+      <c r="F115" s="3" t="n">
+        <v>45909</v>
+      </c>
     </row>
     <row r="116">
       <c r="A116" s="2" t="n">
@@ -2758,6 +3455,12 @@
           <t>15,41€</t>
         </is>
       </c>
+      <c r="E116" t="n">
+        <v>15.41</v>
+      </c>
+      <c r="F116" s="3" t="n">
+        <v>45910</v>
+      </c>
     </row>
     <row r="117">
       <c r="A117" s="2" t="n">
@@ -2778,6 +3481,12 @@
           <t>11,67€</t>
         </is>
       </c>
+      <c r="E117" t="n">
+        <v>11.67</v>
+      </c>
+      <c r="F117" s="3" t="n">
+        <v>45911</v>
+      </c>
     </row>
     <row r="118">
       <c r="A118" s="2" t="n">
@@ -2798,6 +3507,12 @@
           <t>15,41€</t>
         </is>
       </c>
+      <c r="E118" t="n">
+        <v>15.41</v>
+      </c>
+      <c r="F118" s="3" t="n">
+        <v>45912</v>
+      </c>
     </row>
     <row r="119">
       <c r="A119" s="2" t="n">
@@ -2818,6 +3533,12 @@
           <t>15,41€</t>
         </is>
       </c>
+      <c r="E119" t="n">
+        <v>15.41</v>
+      </c>
+      <c r="F119" s="3" t="n">
+        <v>45913</v>
+      </c>
     </row>
     <row r="120">
       <c r="A120" s="2" t="n">
@@ -2838,6 +3559,12 @@
           <t>15,41€</t>
         </is>
       </c>
+      <c r="E120" t="n">
+        <v>15.41</v>
+      </c>
+      <c r="F120" s="3" t="n">
+        <v>45914</v>
+      </c>
     </row>
     <row r="121">
       <c r="A121" s="2" t="n">
@@ -2858,6 +3585,12 @@
           <t>14,75€</t>
         </is>
       </c>
+      <c r="E121" t="n">
+        <v>14.75</v>
+      </c>
+      <c r="F121" s="3" t="n">
+        <v>45915</v>
+      </c>
     </row>
     <row r="122">
       <c r="A122" s="2" t="n">
@@ -2878,6 +3611,12 @@
           <t>11,67€</t>
         </is>
       </c>
+      <c r="E122" t="n">
+        <v>11.67</v>
+      </c>
+      <c r="F122" s="3" t="n">
+        <v>45916</v>
+      </c>
     </row>
     <row r="123">
       <c r="A123" s="2" t="n">
@@ -2898,6 +3637,12 @@
           <t>11,67€</t>
         </is>
       </c>
+      <c r="E123" t="n">
+        <v>11.67</v>
+      </c>
+      <c r="F123" s="3" t="n">
+        <v>45917</v>
+      </c>
     </row>
     <row r="124">
       <c r="A124" s="2" t="n">
@@ -2918,6 +3663,12 @@
           <t>14,00€</t>
         </is>
       </c>
+      <c r="E124" t="n">
+        <v>14</v>
+      </c>
+      <c r="F124" s="3" t="n">
+        <v>45922</v>
+      </c>
     </row>
     <row r="125">
       <c r="A125" s="2" t="n">
@@ -2938,6 +3689,12 @@
           <t>15,41€</t>
         </is>
       </c>
+      <c r="E125" t="n">
+        <v>15.41</v>
+      </c>
+      <c r="F125" s="3" t="n">
+        <v>45923</v>
+      </c>
     </row>
     <row r="126">
       <c r="A126" s="2" t="n">
@@ -2958,6 +3715,12 @@
           <t>11,67€</t>
         </is>
       </c>
+      <c r="E126" t="n">
+        <v>11.67</v>
+      </c>
+      <c r="F126" s="3" t="n">
+        <v>45924</v>
+      </c>
     </row>
     <row r="127">
       <c r="A127" s="2" t="n">
@@ -2978,6 +3741,12 @@
           <t>15,41€</t>
         </is>
       </c>
+      <c r="E127" t="n">
+        <v>15.41</v>
+      </c>
+      <c r="F127" s="3" t="n">
+        <v>45925</v>
+      </c>
     </row>
     <row r="128">
       <c r="A128" s="2" t="n">
@@ -2998,6 +3767,12 @@
           <t>15,41€</t>
         </is>
       </c>
+      <c r="E128" t="n">
+        <v>15.41</v>
+      </c>
+      <c r="F128" s="3" t="n">
+        <v>45926</v>
+      </c>
     </row>
     <row r="129">
       <c r="A129" s="2" t="n">
@@ -3018,6 +3793,12 @@
           <t>15,41€</t>
         </is>
       </c>
+      <c r="E129" t="n">
+        <v>15.41</v>
+      </c>
+      <c r="F129" s="3" t="n">
+        <v>45927</v>
+      </c>
     </row>
     <row r="130">
       <c r="A130" s="2" t="n">
@@ -3038,6 +3819,12 @@
           <t>14,00€</t>
         </is>
       </c>
+      <c r="E130" t="n">
+        <v>14</v>
+      </c>
+      <c r="F130" s="3" t="n">
+        <v>45928</v>
+      </c>
     </row>
     <row r="131">
       <c r="A131" s="2" t="n">
@@ -3058,6 +3845,12 @@
           <t>11,67€</t>
         </is>
       </c>
+      <c r="E131" t="n">
+        <v>11.67</v>
+      </c>
+      <c r="F131" s="3" t="n">
+        <v>45929</v>
+      </c>
     </row>
     <row r="132">
       <c r="A132" s="2" t="n">
@@ -3078,6 +3871,12 @@
           <t>15,41€</t>
         </is>
       </c>
+      <c r="E132" t="n">
+        <v>15.41</v>
+      </c>
+      <c r="F132" s="3" t="n">
+        <v>45930</v>
+      </c>
     </row>
     <row r="133">
       <c r="A133" s="2" t="n">
@@ -3098,6 +3897,12 @@
           <t>11,67€</t>
         </is>
       </c>
+      <c r="E133" t="n">
+        <v>11.67</v>
+      </c>
+      <c r="F133" s="3" t="n">
+        <v>45931</v>
+      </c>
     </row>
     <row r="134">
       <c r="A134" s="2" t="n">
@@ -3118,6 +3923,12 @@
           <t>15,41€</t>
         </is>
       </c>
+      <c r="E134" t="n">
+        <v>15.41</v>
+      </c>
+      <c r="F134" s="3" t="n">
+        <v>45932</v>
+      </c>
     </row>
     <row r="135">
       <c r="A135" s="2" t="n">
@@ -3138,6 +3949,12 @@
           <t>11,67€</t>
         </is>
       </c>
+      <c r="E135" t="n">
+        <v>11.67</v>
+      </c>
+      <c r="F135" s="3" t="n">
+        <v>45933</v>
+      </c>
     </row>
     <row r="136">
       <c r="A136" s="2" t="n">
@@ -3158,6 +3975,12 @@
           <t>15,41€</t>
         </is>
       </c>
+      <c r="E136" t="n">
+        <v>15.41</v>
+      </c>
+      <c r="F136" s="3" t="n">
+        <v>45934</v>
+      </c>
     </row>
     <row r="137">
       <c r="A137" s="2" t="n">
@@ -3178,6 +4001,12 @@
           <t>15,41€</t>
         </is>
       </c>
+      <c r="E137" t="n">
+        <v>15.41</v>
+      </c>
+      <c r="F137" s="3" t="n">
+        <v>45935</v>
+      </c>
     </row>
     <row r="138">
       <c r="A138" s="2" t="n">
@@ -3198,6 +4027,12 @@
           <t>11,67€</t>
         </is>
       </c>
+      <c r="E138" t="n">
+        <v>11.67</v>
+      </c>
+      <c r="F138" s="3" t="n">
+        <v>45936</v>
+      </c>
     </row>
     <row r="139">
       <c r="A139" s="2" t="n">
@@ -3218,6 +4053,12 @@
           <t>15,41€</t>
         </is>
       </c>
+      <c r="E139" t="n">
+        <v>15.41</v>
+      </c>
+      <c r="F139" s="3" t="n">
+        <v>45937</v>
+      </c>
     </row>
     <row r="140">
       <c r="A140" s="2" t="n">
@@ -3238,6 +4079,12 @@
           <t>11,67€</t>
         </is>
       </c>
+      <c r="E140" t="n">
+        <v>11.67</v>
+      </c>
+      <c r="F140" s="3" t="n">
+        <v>45938</v>
+      </c>
     </row>
     <row r="141">
       <c r="A141" s="2" t="n">
@@ -3258,6 +4105,12 @@
           <t>15,41€</t>
         </is>
       </c>
+      <c r="E141" t="n">
+        <v>15.41</v>
+      </c>
+      <c r="F141" s="3" t="n">
+        <v>45939</v>
+      </c>
     </row>
     <row r="142">
       <c r="A142" s="2" t="n">
@@ -3278,6 +4131,12 @@
           <t>14,00€</t>
         </is>
       </c>
+      <c r="E142" t="n">
+        <v>14</v>
+      </c>
+      <c r="F142" s="3" t="n">
+        <v>45940</v>
+      </c>
     </row>
     <row r="143">
       <c r="A143" s="2" t="n">
@@ -3298,6 +4157,12 @@
           <t>15,41€</t>
         </is>
       </c>
+      <c r="E143" t="n">
+        <v>15.41</v>
+      </c>
+      <c r="F143" s="3" t="n">
+        <v>45941</v>
+      </c>
     </row>
     <row r="144">
       <c r="A144" s="2" t="n">
@@ -3318,6 +4183,12 @@
           <t>14,00€</t>
         </is>
       </c>
+      <c r="E144" t="n">
+        <v>14</v>
+      </c>
+      <c r="F144" s="3" t="n">
+        <v>45942</v>
+      </c>
     </row>
     <row r="145">
       <c r="A145" s="2" t="n">
@@ -3338,6 +4209,12 @@
           <t>14,00€</t>
         </is>
       </c>
+      <c r="E145" t="n">
+        <v>14</v>
+      </c>
+      <c r="F145" s="3" t="n">
+        <v>45943</v>
+      </c>
     </row>
     <row r="146">
       <c r="A146" s="2" t="n">
@@ -3358,6 +4235,12 @@
           <t>14,00€</t>
         </is>
       </c>
+      <c r="E146" t="n">
+        <v>14</v>
+      </c>
+      <c r="F146" s="3" t="n">
+        <v>45944</v>
+      </c>
     </row>
     <row r="147">
       <c r="A147" s="2" t="n">
@@ -3378,6 +4261,12 @@
           <t>14,00€</t>
         </is>
       </c>
+      <c r="E147" t="n">
+        <v>14</v>
+      </c>
+      <c r="F147" s="3" t="n">
+        <v>45945</v>
+      </c>
     </row>
     <row r="148">
       <c r="A148" s="2" t="n">
@@ -3398,6 +4287,12 @@
           <t>14,00€</t>
         </is>
       </c>
+      <c r="E148" t="n">
+        <v>14</v>
+      </c>
+      <c r="F148" s="3" t="n">
+        <v>45946</v>
+      </c>
     </row>
     <row r="149">
       <c r="A149" s="2" t="n">
@@ -3418,6 +4313,12 @@
           <t>14,00€</t>
         </is>
       </c>
+      <c r="E149" t="n">
+        <v>14</v>
+      </c>
+      <c r="F149" s="3" t="n">
+        <v>45947</v>
+      </c>
     </row>
     <row r="150">
       <c r="A150" s="2" t="n">
@@ -3438,6 +4339,12 @@
           <t>14,00€</t>
         </is>
       </c>
+      <c r="E150" t="n">
+        <v>14</v>
+      </c>
+      <c r="F150" s="3" t="n">
+        <v>45950</v>
+      </c>
     </row>
     <row r="151">
       <c r="A151" s="2" t="n">
@@ -3458,6 +4365,12 @@
           <t>14,00€</t>
         </is>
       </c>
+      <c r="E151" t="n">
+        <v>14</v>
+      </c>
+      <c r="F151" s="3" t="n">
+        <v>45951</v>
+      </c>
     </row>
     <row r="152">
       <c r="A152" s="2" t="n">
@@ -3478,6 +4391,12 @@
           <t>15,41€</t>
         </is>
       </c>
+      <c r="E152" t="n">
+        <v>15.41</v>
+      </c>
+      <c r="F152" s="3" t="n">
+        <v>45952</v>
+      </c>
     </row>
     <row r="153">
       <c r="A153" s="2" t="n">
@@ -3498,6 +4417,12 @@
           <t>14,00€</t>
         </is>
       </c>
+      <c r="E153" t="n">
+        <v>14</v>
+      </c>
+      <c r="F153" s="3" t="n">
+        <v>45953</v>
+      </c>
     </row>
     <row r="154">
       <c r="A154" s="2" t="n">
@@ -3518,6 +4443,12 @@
           <t>14,00€</t>
         </is>
       </c>
+      <c r="E154" t="n">
+        <v>14</v>
+      </c>
+      <c r="F154" s="3" t="n">
+        <v>45954</v>
+      </c>
     </row>
     <row r="155">
       <c r="A155" s="2" t="n">
@@ -3538,6 +4469,12 @@
           <t>15,41€</t>
         </is>
       </c>
+      <c r="E155" t="n">
+        <v>15.41</v>
+      </c>
+      <c r="F155" s="3" t="n">
+        <v>45955</v>
+      </c>
     </row>
     <row r="156">
       <c r="A156" s="2" t="n">
@@ -3558,6 +4495,12 @@
           <t>14,00€</t>
         </is>
       </c>
+      <c r="E156" t="n">
+        <v>14</v>
+      </c>
+      <c r="F156" s="3" t="n">
+        <v>45956</v>
+      </c>
     </row>
     <row r="157">
       <c r="A157" s="2" t="n">
@@ -3578,6 +4521,12 @@
           <t>14,00€</t>
         </is>
       </c>
+      <c r="E157" t="n">
+        <v>14</v>
+      </c>
+      <c r="F157" s="3" t="n">
+        <v>45957</v>
+      </c>
     </row>
     <row r="158">
       <c r="A158" s="2" t="n">
@@ -3598,6 +4547,12 @@
           <t>14,00€</t>
         </is>
       </c>
+      <c r="E158" t="n">
+        <v>14</v>
+      </c>
+      <c r="F158" s="3" t="n">
+        <v>45958</v>
+      </c>
     </row>
     <row r="159">
       <c r="A159" s="2" t="n">
@@ -3618,6 +4573,12 @@
           <t>14,00€</t>
         </is>
       </c>
+      <c r="E159" t="n">
+        <v>14</v>
+      </c>
+      <c r="F159" s="3" t="n">
+        <v>45958</v>
+      </c>
     </row>
     <row r="160">
       <c r="A160" s="2" t="n">
@@ -3638,10 +4599,16 @@
           <t>14,00€</t>
         </is>
       </c>
+      <c r="E160" t="n">
+        <v>14</v>
+      </c>
+      <c r="F160" s="3" t="n">
+        <v>45958</v>
+      </c>
     </row>
     <row r="161">
       <c r="A161" s="2" t="n">
-        <v>45964.36348250412</v>
+        <v>45964.3634825</v>
       </c>
       <c r="B161" t="inlineStr">
         <is>
@@ -3658,6 +4625,710 @@
           <t>14,00€</t>
         </is>
       </c>
+      <c r="E161" t="n">
+        <v>14</v>
+      </c>
+      <c r="F161" s="3" t="n">
+        <v>45964</v>
+      </c>
+    </row>
+    <row r="162">
+      <c r="A162" s="2" t="n">
+        <v>45966.36921778935</v>
+      </c>
+      <c r="B162" t="inlineStr">
+        <is>
+          <t>CREATINA MONOHIDRATO EN POLVO</t>
+        </is>
+      </c>
+      <c r="C162" t="inlineStr">
+        <is>
+          <t>1Kg</t>
+        </is>
+      </c>
+      <c r="D162" t="inlineStr">
+        <is>
+          <t>14,00€</t>
+        </is>
+      </c>
+      <c r="E162" t="n">
+        <v>14</v>
+      </c>
+      <c r="F162" s="3" t="n">
+        <v>45966</v>
+      </c>
+    </row>
+    <row r="163">
+      <c r="A163" s="2" t="n">
+        <v>45966.39764065972</v>
+      </c>
+      <c r="B163" t="inlineStr">
+        <is>
+          <t>CREATINA MONOHIDRATO EN POLVO</t>
+        </is>
+      </c>
+      <c r="C163" t="inlineStr">
+        <is>
+          <t>1Kg</t>
+        </is>
+      </c>
+      <c r="D163" t="inlineStr">
+        <is>
+          <t>14,00€</t>
+        </is>
+      </c>
+      <c r="E163" t="n">
+        <v>14</v>
+      </c>
+      <c r="F163" s="3" t="n">
+        <v>45966</v>
+      </c>
+    </row>
+    <row r="164">
+      <c r="A164" s="2" t="n">
+        <v>45966.45845660879</v>
+      </c>
+      <c r="B164" t="inlineStr">
+        <is>
+          <t>CREATINA MONOHIDRATO EN POLVO</t>
+        </is>
+      </c>
+      <c r="C164" t="inlineStr">
+        <is>
+          <t>1Kg</t>
+        </is>
+      </c>
+      <c r="D164" t="inlineStr">
+        <is>
+          <t>14,00€</t>
+        </is>
+      </c>
+      <c r="E164" t="n">
+        <v>14</v>
+      </c>
+      <c r="F164" s="3" t="n">
+        <v>45966</v>
+      </c>
+    </row>
+    <row r="165">
+      <c r="A165" s="2" t="n">
+        <v>45967.45865304398</v>
+      </c>
+      <c r="B165" t="inlineStr">
+        <is>
+          <t>CREATINA MONOHIDRATO EN POLVO</t>
+        </is>
+      </c>
+      <c r="C165" t="inlineStr">
+        <is>
+          <t>1Kg</t>
+        </is>
+      </c>
+      <c r="D165" t="inlineStr">
+        <is>
+          <t>14,00€</t>
+        </is>
+      </c>
+      <c r="E165" t="n">
+        <v>14</v>
+      </c>
+      <c r="F165" s="3" t="n">
+        <v>45967</v>
+      </c>
+    </row>
+    <row r="166">
+      <c r="A166" s="2" t="n">
+        <v>45968.45855202546</v>
+      </c>
+      <c r="B166" t="inlineStr">
+        <is>
+          <t>CREATINA MONOHIDRATO EN POLVO</t>
+        </is>
+      </c>
+      <c r="C166" t="inlineStr">
+        <is>
+          <t>1Kg</t>
+        </is>
+      </c>
+      <c r="D166" t="inlineStr">
+        <is>
+          <t>15,41€</t>
+        </is>
+      </c>
+      <c r="E166" t="n">
+        <v>15.41</v>
+      </c>
+      <c r="F166" s="3" t="n">
+        <v>45968</v>
+      </c>
+    </row>
+    <row r="167">
+      <c r="A167" s="2" t="n">
+        <v>45969.45851944444</v>
+      </c>
+      <c r="B167" t="inlineStr">
+        <is>
+          <t>CREATINA MONOHIDRATO EN POLVO</t>
+        </is>
+      </c>
+      <c r="C167" t="inlineStr">
+        <is>
+          <t>1Kg</t>
+        </is>
+      </c>
+      <c r="D167" t="inlineStr">
+        <is>
+          <t>15,41€</t>
+        </is>
+      </c>
+      <c r="E167" t="n">
+        <v>15.41</v>
+      </c>
+      <c r="F167" s="3" t="n">
+        <v>45969</v>
+      </c>
+    </row>
+    <row r="168">
+      <c r="A168" s="2" t="n">
+        <v>45970.45851274305</v>
+      </c>
+      <c r="B168" t="inlineStr">
+        <is>
+          <t>CREATINA MONOHIDRATO EN POLVO</t>
+        </is>
+      </c>
+      <c r="C168" t="inlineStr">
+        <is>
+          <t>1Kg</t>
+        </is>
+      </c>
+      <c r="D168" t="inlineStr">
+        <is>
+          <t>14,00€</t>
+        </is>
+      </c>
+      <c r="E168" t="n">
+        <v>14</v>
+      </c>
+      <c r="F168" s="3" t="n">
+        <v>45970</v>
+      </c>
+    </row>
+    <row r="169">
+      <c r="A169" s="2" t="n">
+        <v>45971.45852486111</v>
+      </c>
+      <c r="B169" t="inlineStr">
+        <is>
+          <t>CREATINA MONOHIDRATO EN POLVO</t>
+        </is>
+      </c>
+      <c r="C169" t="inlineStr">
+        <is>
+          <t>1Kg</t>
+        </is>
+      </c>
+      <c r="D169" t="inlineStr">
+        <is>
+          <t>14,00€</t>
+        </is>
+      </c>
+      <c r="E169" t="n">
+        <v>14</v>
+      </c>
+      <c r="F169" s="3" t="n">
+        <v>45971</v>
+      </c>
+    </row>
+    <row r="170">
+      <c r="A170" s="2" t="n">
+        <v>45972.45852538195</v>
+      </c>
+      <c r="B170" t="inlineStr">
+        <is>
+          <t>CREATINA MONOHIDRATO EN POLVO</t>
+        </is>
+      </c>
+      <c r="C170" t="inlineStr">
+        <is>
+          <t>1Kg</t>
+        </is>
+      </c>
+      <c r="D170" t="inlineStr">
+        <is>
+          <t>14,00€</t>
+        </is>
+      </c>
+      <c r="E170" t="n">
+        <v>14</v>
+      </c>
+      <c r="F170" s="3" t="n">
+        <v>45972</v>
+      </c>
+    </row>
+    <row r="171">
+      <c r="A171" s="2" t="n">
+        <v>45973.4585581713</v>
+      </c>
+      <c r="B171" t="inlineStr">
+        <is>
+          <t>CREATINA MONOHIDRATO EN POLVO</t>
+        </is>
+      </c>
+      <c r="C171" t="inlineStr">
+        <is>
+          <t>1Kg</t>
+        </is>
+      </c>
+      <c r="D171" t="inlineStr">
+        <is>
+          <t>15,41€</t>
+        </is>
+      </c>
+      <c r="E171" t="n">
+        <v>15.41</v>
+      </c>
+      <c r="F171" s="3" t="n">
+        <v>45973</v>
+      </c>
+    </row>
+    <row r="172">
+      <c r="A172" s="2" t="n">
+        <v>45974.45852885416</v>
+      </c>
+      <c r="B172" t="inlineStr">
+        <is>
+          <t>CREATINA MONOHIDRATO EN POLVO</t>
+        </is>
+      </c>
+      <c r="C172" t="inlineStr">
+        <is>
+          <t>1Kg</t>
+        </is>
+      </c>
+      <c r="D172" t="inlineStr">
+        <is>
+          <t>14,00€</t>
+        </is>
+      </c>
+      <c r="E172" t="n">
+        <v>14</v>
+      </c>
+      <c r="F172" s="3" t="n">
+        <v>45974</v>
+      </c>
+    </row>
+    <row r="173">
+      <c r="A173" s="2" t="n">
+        <v>45978.45852159723</v>
+      </c>
+      <c r="B173" t="inlineStr">
+        <is>
+          <t>CREATINA MONOHIDRATO EN POLVO</t>
+        </is>
+      </c>
+      <c r="C173" t="inlineStr">
+        <is>
+          <t>1Kg</t>
+        </is>
+      </c>
+      <c r="D173" t="inlineStr">
+        <is>
+          <t>14,00€</t>
+        </is>
+      </c>
+      <c r="E173" t="n">
+        <v>14</v>
+      </c>
+      <c r="F173" s="3" t="n">
+        <v>45978</v>
+      </c>
+    </row>
+    <row r="174">
+      <c r="A174" s="2" t="n">
+        <v>45979.45851483796</v>
+      </c>
+      <c r="B174" t="inlineStr">
+        <is>
+          <t>CREATINA MONOHIDRATO EN POLVO</t>
+        </is>
+      </c>
+      <c r="C174" t="inlineStr">
+        <is>
+          <t>1Kg</t>
+        </is>
+      </c>
+      <c r="D174" t="inlineStr">
+        <is>
+          <t>14,00€</t>
+        </is>
+      </c>
+      <c r="E174" t="n">
+        <v>14</v>
+      </c>
+      <c r="F174" s="3" t="n">
+        <v>45979</v>
+      </c>
+    </row>
+    <row r="175">
+      <c r="A175" s="2" t="n">
+        <v>45980.45851055555</v>
+      </c>
+      <c r="B175" t="inlineStr">
+        <is>
+          <t>CREATINA MONOHIDRATO EN POLVO</t>
+        </is>
+      </c>
+      <c r="C175" t="inlineStr">
+        <is>
+          <t>1Kg</t>
+        </is>
+      </c>
+      <c r="D175" t="inlineStr">
+        <is>
+          <t>15,41€</t>
+        </is>
+      </c>
+      <c r="E175" t="n">
+        <v>15.41</v>
+      </c>
+      <c r="F175" s="3" t="n">
+        <v>45980</v>
+      </c>
+    </row>
+    <row r="176">
+      <c r="A176" s="2" t="n">
+        <v>45981.45850697916</v>
+      </c>
+      <c r="B176" t="inlineStr">
+        <is>
+          <t>CREATINA MONOHIDRATO EN POLVO</t>
+        </is>
+      </c>
+      <c r="C176" t="inlineStr">
+        <is>
+          <t>1Kg</t>
+        </is>
+      </c>
+      <c r="D176" t="inlineStr">
+        <is>
+          <t>14,00€</t>
+        </is>
+      </c>
+      <c r="E176" t="n">
+        <v>14</v>
+      </c>
+      <c r="F176" s="3" t="n">
+        <v>45981</v>
+      </c>
+    </row>
+    <row r="177">
+      <c r="A177" s="2" t="n">
+        <v>45985.45854479167</v>
+      </c>
+      <c r="B177" t="inlineStr">
+        <is>
+          <t>CREATINA MONOHIDRATO EN POLVO</t>
+        </is>
+      </c>
+      <c r="C177" t="inlineStr">
+        <is>
+          <t>1Kg</t>
+        </is>
+      </c>
+      <c r="D177" t="inlineStr">
+        <is>
+          <t>10,90€</t>
+        </is>
+      </c>
+      <c r="E177" t="n">
+        <v>10.9</v>
+      </c>
+      <c r="F177" s="3" t="n">
+        <v>45985</v>
+      </c>
+    </row>
+    <row r="178">
+      <c r="A178" s="2" t="n">
+        <v>45986.39178425926</v>
+      </c>
+      <c r="B178" t="inlineStr">
+        <is>
+          <t>CREATINA MONOHIDRATO EN POLVO</t>
+        </is>
+      </c>
+      <c r="C178" t="inlineStr">
+        <is>
+          <t>1Kg</t>
+        </is>
+      </c>
+      <c r="D178" t="inlineStr">
+        <is>
+          <t>10,90€</t>
+        </is>
+      </c>
+      <c r="E178" t="n">
+        <v>10.9</v>
+      </c>
+      <c r="F178" s="3" t="n">
+        <v>45986</v>
+      </c>
+    </row>
+    <row r="179">
+      <c r="A179" s="2" t="n">
+        <v>45986.40508719908</v>
+      </c>
+      <c r="B179" t="inlineStr">
+        <is>
+          <t>CREATINA MONOHIDRATO EN POLVO</t>
+        </is>
+      </c>
+      <c r="C179" t="inlineStr">
+        <is>
+          <t>1Kg</t>
+        </is>
+      </c>
+      <c r="D179" t="inlineStr">
+        <is>
+          <t>10,90€</t>
+        </is>
+      </c>
+      <c r="E179" t="n">
+        <v>10.9</v>
+      </c>
+      <c r="F179" s="3" t="n">
+        <v>45986</v>
+      </c>
+    </row>
+    <row r="180">
+      <c r="A180" s="2" t="n">
+        <v>45986.40571390047</v>
+      </c>
+      <c r="B180" t="inlineStr">
+        <is>
+          <t>CREATINA MONOHIDRATO EN POLVO</t>
+        </is>
+      </c>
+      <c r="C180" t="inlineStr">
+        <is>
+          <t>1Kg</t>
+        </is>
+      </c>
+      <c r="D180" t="inlineStr">
+        <is>
+          <t>10,90€</t>
+        </is>
+      </c>
+      <c r="E180" t="n">
+        <v>10.9</v>
+      </c>
+      <c r="F180" s="3" t="n">
+        <v>45986</v>
+      </c>
+    </row>
+    <row r="181">
+      <c r="A181" s="2" t="n">
+        <v>45986.40635800926</v>
+      </c>
+      <c r="B181" t="inlineStr">
+        <is>
+          <t>CREATINA MONOHIDRATO EN POLVO</t>
+        </is>
+      </c>
+      <c r="C181" t="inlineStr">
+        <is>
+          <t>1Kg</t>
+        </is>
+      </c>
+      <c r="D181" t="inlineStr">
+        <is>
+          <t>10,90€</t>
+        </is>
+      </c>
+      <c r="E181" t="n">
+        <v>10.9</v>
+      </c>
+      <c r="F181" s="3" t="n">
+        <v>45986</v>
+      </c>
+    </row>
+    <row r="182">
+      <c r="A182" s="2" t="n">
+        <v>45986.40844466435</v>
+      </c>
+      <c r="B182" t="inlineStr">
+        <is>
+          <t>CREATINA MONOHIDRATO EN POLVO</t>
+        </is>
+      </c>
+      <c r="C182" t="inlineStr">
+        <is>
+          <t>1Kg</t>
+        </is>
+      </c>
+      <c r="D182" t="inlineStr">
+        <is>
+          <t>10,90€</t>
+        </is>
+      </c>
+      <c r="E182" t="n">
+        <v>10.9</v>
+      </c>
+      <c r="F182" s="3" t="n">
+        <v>45986</v>
+      </c>
+    </row>
+    <row r="183">
+      <c r="A183" s="2" t="n">
+        <v>45986.41843248843</v>
+      </c>
+      <c r="B183" t="inlineStr">
+        <is>
+          <t>CREATINA MONOHIDRATO EN POLVO</t>
+        </is>
+      </c>
+      <c r="C183" t="inlineStr">
+        <is>
+          <t>1Kg</t>
+        </is>
+      </c>
+      <c r="D183" t="inlineStr">
+        <is>
+          <t>10,90€</t>
+        </is>
+      </c>
+      <c r="E183" t="n">
+        <v>10.9</v>
+      </c>
+      <c r="F183" s="3" t="n">
+        <v>45986</v>
+      </c>
+    </row>
+    <row r="184">
+      <c r="A184" s="2" t="n">
+        <v>45986.41967928241</v>
+      </c>
+      <c r="B184" t="inlineStr">
+        <is>
+          <t>CREATINA MONOHIDRATO EN POLVO</t>
+        </is>
+      </c>
+      <c r="C184" t="inlineStr">
+        <is>
+          <t>1Kg</t>
+        </is>
+      </c>
+      <c r="D184" t="inlineStr">
+        <is>
+          <t>10,90€</t>
+        </is>
+      </c>
+      <c r="E184" t="n">
+        <v>10.9</v>
+      </c>
+      <c r="F184" s="3" t="n">
+        <v>45986</v>
+      </c>
+    </row>
+    <row r="185">
+      <c r="A185" s="2" t="n">
+        <v>45986.42274222222</v>
+      </c>
+      <c r="B185" t="inlineStr">
+        <is>
+          <t>CREATINA MONOHIDRATO EN POLVO</t>
+        </is>
+      </c>
+      <c r="C185" t="inlineStr">
+        <is>
+          <t>1Kg</t>
+        </is>
+      </c>
+      <c r="D185" t="inlineStr">
+        <is>
+          <t>10,90€</t>
+        </is>
+      </c>
+      <c r="E185" t="n">
+        <v>10.9</v>
+      </c>
+      <c r="F185" s="3" t="n">
+        <v>45986</v>
+      </c>
+    </row>
+    <row r="186">
+      <c r="A186" s="2" t="n">
+        <v>45986.42965295139</v>
+      </c>
+      <c r="B186" t="inlineStr">
+        <is>
+          <t>CREATINA MONOHIDRATO EN POLVO</t>
+        </is>
+      </c>
+      <c r="C186" t="inlineStr">
+        <is>
+          <t>1Kg</t>
+        </is>
+      </c>
+      <c r="D186" t="inlineStr">
+        <is>
+          <t>10,90€</t>
+        </is>
+      </c>
+      <c r="E186" t="n">
+        <v>10.9</v>
+      </c>
+      <c r="F186" s="3" t="n">
+        <v>45986</v>
+      </c>
+    </row>
+    <row r="187">
+      <c r="A187" s="2" t="n">
+        <v>45986.43291543981</v>
+      </c>
+      <c r="B187" t="inlineStr">
+        <is>
+          <t>CREATINA MONOHIDRATO EN POLVO</t>
+        </is>
+      </c>
+      <c r="C187" t="inlineStr">
+        <is>
+          <t>1Kg</t>
+        </is>
+      </c>
+      <c r="D187" t="inlineStr">
+        <is>
+          <t>10,90€</t>
+        </is>
+      </c>
+      <c r="E187" t="n">
+        <v>10.9</v>
+      </c>
+      <c r="F187" s="3" t="n">
+        <v>45986</v>
+      </c>
+    </row>
+    <row r="188">
+      <c r="A188" s="2" t="n">
+        <v>45986.43554897553</v>
+      </c>
+      <c r="B188" t="inlineStr">
+        <is>
+          <t>CREATINA MONOHIDRATO EN POLVO</t>
+        </is>
+      </c>
+      <c r="C188" t="inlineStr">
+        <is>
+          <t>1Kg</t>
+        </is>
+      </c>
+      <c r="D188" t="inlineStr">
+        <is>
+          <t>10,90€</t>
+        </is>
+      </c>
+      <c r="E188" t="inlineStr"/>
+      <c r="F188" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
arreglo error de main.py para ejecucion automatica
</commit_message>
<xml_diff>
--- a/data/precios_creatina.xlsx
+++ b/data/precios_creatina.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F188"/>
+  <dimension ref="A1:F197"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5310,7 +5310,7 @@
     </row>
     <row r="188">
       <c r="A188" s="2" t="n">
-        <v>45986.43554897553</v>
+        <v>45986.43554896991</v>
       </c>
       <c r="B188" t="inlineStr">
         <is>
@@ -5327,8 +5327,242 @@
           <t>10,90€</t>
         </is>
       </c>
-      <c r="E188" t="inlineStr"/>
-      <c r="F188" t="inlineStr"/>
+      <c r="E188" t="n">
+        <v>10.9</v>
+      </c>
+      <c r="F188" s="3" t="n">
+        <v>45986</v>
+      </c>
+    </row>
+    <row r="189">
+      <c r="A189" s="2" t="n">
+        <v>45986.48648068287</v>
+      </c>
+      <c r="B189" t="inlineStr">
+        <is>
+          <t>CREATINA MONOHIDRATO EN POLVO</t>
+        </is>
+      </c>
+      <c r="C189" t="inlineStr">
+        <is>
+          <t>1Kg</t>
+        </is>
+      </c>
+      <c r="D189" t="inlineStr">
+        <is>
+          <t>10,90€</t>
+        </is>
+      </c>
+      <c r="E189" t="n">
+        <v>10.9</v>
+      </c>
+      <c r="F189" s="3" t="n">
+        <v>45986</v>
+      </c>
+    </row>
+    <row r="190">
+      <c r="A190" s="2" t="n">
+        <v>45986.49726113426</v>
+      </c>
+      <c r="B190" t="inlineStr">
+        <is>
+          <t>CREATINA MONOHIDRATO EN POLVO</t>
+        </is>
+      </c>
+      <c r="C190" t="inlineStr">
+        <is>
+          <t>1Kg</t>
+        </is>
+      </c>
+      <c r="D190" t="inlineStr">
+        <is>
+          <t>10,90€</t>
+        </is>
+      </c>
+      <c r="E190" t="n">
+        <v>10.9</v>
+      </c>
+      <c r="F190" s="3" t="n">
+        <v>45986</v>
+      </c>
+    </row>
+    <row r="191">
+      <c r="A191" s="2" t="n">
+        <v>45987.42159631944</v>
+      </c>
+      <c r="B191" t="inlineStr">
+        <is>
+          <t>CREATINA MONOHIDRATO EN POLVO</t>
+        </is>
+      </c>
+      <c r="C191" t="inlineStr">
+        <is>
+          <t>1Kg</t>
+        </is>
+      </c>
+      <c r="D191" t="inlineStr">
+        <is>
+          <t>10,90€</t>
+        </is>
+      </c>
+      <c r="E191" t="n">
+        <v>10.9</v>
+      </c>
+      <c r="F191" s="3" t="n">
+        <v>45987</v>
+      </c>
+    </row>
+    <row r="192">
+      <c r="A192" s="2" t="n">
+        <v>45987.42376754629</v>
+      </c>
+      <c r="B192" t="inlineStr">
+        <is>
+          <t>CREATINA MONOHIDRATO EN POLVO</t>
+        </is>
+      </c>
+      <c r="C192" t="inlineStr">
+        <is>
+          <t>1Kg</t>
+        </is>
+      </c>
+      <c r="D192" t="inlineStr">
+        <is>
+          <t>10,90€</t>
+        </is>
+      </c>
+      <c r="E192" t="n">
+        <v>10.9</v>
+      </c>
+      <c r="F192" s="3" t="n">
+        <v>45987</v>
+      </c>
+    </row>
+    <row r="193">
+      <c r="A193" s="2" t="n">
+        <v>45987.42439525463</v>
+      </c>
+      <c r="B193" t="inlineStr">
+        <is>
+          <t>CREATINA MONOHIDRATO EN POLVO</t>
+        </is>
+      </c>
+      <c r="C193" t="inlineStr">
+        <is>
+          <t>1Kg</t>
+        </is>
+      </c>
+      <c r="D193" t="inlineStr">
+        <is>
+          <t>10,90€</t>
+        </is>
+      </c>
+      <c r="E193" t="n">
+        <v>10.9</v>
+      </c>
+      <c r="F193" s="3" t="n">
+        <v>45987</v>
+      </c>
+    </row>
+    <row r="194">
+      <c r="A194" s="2" t="n">
+        <v>45987.42467140046</v>
+      </c>
+      <c r="B194" t="inlineStr">
+        <is>
+          <t>CREATINA MONOHIDRATO EN POLVO</t>
+        </is>
+      </c>
+      <c r="C194" t="inlineStr">
+        <is>
+          <t>1Kg</t>
+        </is>
+      </c>
+      <c r="D194" t="inlineStr">
+        <is>
+          <t>10,90€</t>
+        </is>
+      </c>
+      <c r="E194" t="n">
+        <v>10.9</v>
+      </c>
+      <c r="F194" s="3" t="n">
+        <v>45987</v>
+      </c>
+    </row>
+    <row r="195">
+      <c r="A195" s="2" t="n">
+        <v>45987.4262396875</v>
+      </c>
+      <c r="B195" t="inlineStr">
+        <is>
+          <t>CREATINA MONOHIDRATO EN POLVO</t>
+        </is>
+      </c>
+      <c r="C195" t="inlineStr">
+        <is>
+          <t>1Kg</t>
+        </is>
+      </c>
+      <c r="D195" t="inlineStr">
+        <is>
+          <t>10,90€</t>
+        </is>
+      </c>
+      <c r="E195" t="n">
+        <v>10.9</v>
+      </c>
+      <c r="F195" s="3" t="n">
+        <v>45987</v>
+      </c>
+    </row>
+    <row r="196">
+      <c r="A196" s="2" t="n">
+        <v>45987.42668586806</v>
+      </c>
+      <c r="B196" t="inlineStr">
+        <is>
+          <t>CREATINA MONOHIDRATO EN POLVO</t>
+        </is>
+      </c>
+      <c r="C196" t="inlineStr">
+        <is>
+          <t>1Kg</t>
+        </is>
+      </c>
+      <c r="D196" t="inlineStr">
+        <is>
+          <t>10,90€</t>
+        </is>
+      </c>
+      <c r="E196" t="n">
+        <v>10.9</v>
+      </c>
+      <c r="F196" s="3" t="n">
+        <v>45987</v>
+      </c>
+    </row>
+    <row r="197">
+      <c r="A197" s="2" t="n">
+        <v>45987.42764274263</v>
+      </c>
+      <c r="B197" t="inlineStr">
+        <is>
+          <t>CREATINA MONOHIDRATO EN POLVO</t>
+        </is>
+      </c>
+      <c r="C197" t="inlineStr">
+        <is>
+          <t>1Kg</t>
+        </is>
+      </c>
+      <c r="D197" t="inlineStr">
+        <is>
+          <t>10,90€</t>
+        </is>
+      </c>
+      <c r="E197" t="inlineStr"/>
+      <c r="F197" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>